<commit_message>
new calc for J
</commit_message>
<xml_diff>
--- a/CSV/meas0calc.xlsx
+++ b/CSV/meas0calc.xlsx
@@ -8,14 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ditte\aauRepo\esd7_git\3Dprinter-BLDC-control\CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1D440193-2C3B-4DD7-BFD1-3B75EF60EBEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04019008-D2D8-497B-834B-9095D22D3D06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{E87BC9E1-8444-4612-85BE-F946921EBAC5}"/>
   </bookViews>
   <sheets>
     <sheet name="meas0calc" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -694,556 +707,553 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="184"/>
                 <c:pt idx="0">
-                  <c:v>2E-3</c:v>
+                  <c:v>1.2E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.1999999999999999E-2</c:v>
+                  <c:v>2.4E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.1999999999999996E-2</c:v>
+                  <c:v>3.6000000000000004E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.2E-2</c:v>
+                  <c:v>4.8000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.2000000000000003E-2</c:v>
+                  <c:v>0.06</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.10200000000000001</c:v>
+                  <c:v>7.1999999999999995E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.12200000000000001</c:v>
+                  <c:v>8.3999999999999991E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.14200000000000002</c:v>
+                  <c:v>9.5999999999999988E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.16200000000000001</c:v>
+                  <c:v>0.10799999999999998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.182</c:v>
+                  <c:v>0.11999999999999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.20199999999999999</c:v>
+                  <c:v>0.13199999999999998</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.22199999999999998</c:v>
+                  <c:v>0.14399999999999999</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.24199999999999997</c:v>
+                  <c:v>0.156</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.26199999999999996</c:v>
+                  <c:v>0.16800000000000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.28199999999999997</c:v>
+                  <c:v>0.18000000000000002</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.30199999999999999</c:v>
+                  <c:v>0.19200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.32200000000000001</c:v>
+                  <c:v>0.20400000000000004</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.34200000000000003</c:v>
+                  <c:v>0.21600000000000005</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.36200000000000004</c:v>
+                  <c:v>0.22800000000000006</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.38200000000000006</c:v>
+                  <c:v>0.24000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.40200000000000008</c:v>
+                  <c:v>0.25200000000000006</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.4220000000000001</c:v>
+                  <c:v>0.26400000000000007</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.44200000000000012</c:v>
+                  <c:v>0.27600000000000008</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.46200000000000013</c:v>
+                  <c:v>0.28800000000000009</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.48200000000000015</c:v>
+                  <c:v>0.3000000000000001</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.50200000000000011</c:v>
+                  <c:v>0.31200000000000011</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.52200000000000013</c:v>
+                  <c:v>0.32400000000000012</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.54200000000000015</c:v>
+                  <c:v>0.33600000000000013</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.56200000000000017</c:v>
+                  <c:v>0.34800000000000014</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.58200000000000018</c:v>
+                  <c:v>0.36000000000000015</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.6020000000000002</c:v>
+                  <c:v>0.37200000000000016</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.62200000000000022</c:v>
+                  <c:v>0.38400000000000017</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.64200000000000024</c:v>
+                  <c:v>0.39600000000000019</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.66200000000000025</c:v>
+                  <c:v>0.4080000000000002</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.68200000000000027</c:v>
+                  <c:v>0.42000000000000021</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.70200000000000029</c:v>
+                  <c:v>0.43200000000000022</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.72200000000000031</c:v>
+                  <c:v>0.44400000000000023</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.74200000000000033</c:v>
+                  <c:v>0.45600000000000024</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.76200000000000034</c:v>
+                  <c:v>0.46800000000000025</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.78200000000000036</c:v>
+                  <c:v>0.48000000000000026</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.80200000000000038</c:v>
+                  <c:v>0.49200000000000027</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.8220000000000004</c:v>
+                  <c:v>0.50400000000000023</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.84200000000000041</c:v>
+                  <c:v>0.51600000000000024</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.86200000000000043</c:v>
+                  <c:v>0.52800000000000025</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.88200000000000045</c:v>
+                  <c:v>0.54000000000000026</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.90200000000000047</c:v>
+                  <c:v>0.55200000000000027</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.92200000000000049</c:v>
+                  <c:v>0.56400000000000028</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.9420000000000005</c:v>
+                  <c:v>0.57600000000000029</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.96200000000000052</c:v>
+                  <c:v>0.5880000000000003</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.98200000000000054</c:v>
+                  <c:v>0.60000000000000031</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>1.0020000000000004</c:v>
+                  <c:v>0.61200000000000032</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>1.0220000000000005</c:v>
+                  <c:v>0.62400000000000033</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>1.0420000000000005</c:v>
+                  <c:v>0.63600000000000034</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>1.0620000000000005</c:v>
+                  <c:v>0.64800000000000035</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>1.0820000000000005</c:v>
+                  <c:v>0.66000000000000036</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>1.1020000000000005</c:v>
+                  <c:v>0.67200000000000037</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>1.1220000000000006</c:v>
+                  <c:v>0.68400000000000039</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>1.1420000000000006</c:v>
+                  <c:v>0.6960000000000004</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>1.1620000000000006</c:v>
+                  <c:v>0.70800000000000041</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>1.1820000000000006</c:v>
+                  <c:v>0.72000000000000042</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>1.2020000000000006</c:v>
+                  <c:v>0.73200000000000043</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>1.2220000000000006</c:v>
+                  <c:v>0.74400000000000044</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>1.2420000000000007</c:v>
+                  <c:v>0.75600000000000045</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>1.2620000000000007</c:v>
+                  <c:v>0.76800000000000046</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>1.2820000000000007</c:v>
+                  <c:v>0.78000000000000047</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>1.3020000000000007</c:v>
+                  <c:v>0.79200000000000048</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>1.3220000000000007</c:v>
+                  <c:v>0.80400000000000049</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>1.3420000000000007</c:v>
+                  <c:v>0.8160000000000005</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>1.3620000000000008</c:v>
+                  <c:v>0.82800000000000051</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>1.3820000000000008</c:v>
+                  <c:v>0.84000000000000052</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>1.4020000000000008</c:v>
+                  <c:v>0.85200000000000053</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>1.4220000000000008</c:v>
+                  <c:v>0.86400000000000055</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>1.4420000000000008</c:v>
+                  <c:v>0.87600000000000056</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>1.4620000000000009</c:v>
+                  <c:v>0.88800000000000057</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>1.4820000000000009</c:v>
+                  <c:v>0.90000000000000058</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>1.5020000000000009</c:v>
+                  <c:v>0.91200000000000059</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>1.5220000000000009</c:v>
+                  <c:v>0.9240000000000006</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>1.5420000000000009</c:v>
+                  <c:v>0.93600000000000061</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>1.5620000000000009</c:v>
+                  <c:v>0.94800000000000062</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>1.582000000000001</c:v>
+                  <c:v>0.96000000000000063</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>1.602000000000001</c:v>
+                  <c:v>0.97200000000000064</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>1.622000000000001</c:v>
+                  <c:v>0.98400000000000065</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>1.642000000000001</c:v>
+                  <c:v>0.99600000000000066</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>1.662000000000001</c:v>
+                  <c:v>1.0080000000000007</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>1.682000000000001</c:v>
+                  <c:v>1.0200000000000007</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>1.7020000000000011</c:v>
+                  <c:v>1.0320000000000007</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>1.7220000000000011</c:v>
+                  <c:v>1.0440000000000007</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>1.7420000000000011</c:v>
+                  <c:v>1.0560000000000007</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>1.7620000000000011</c:v>
+                  <c:v>1.0680000000000007</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>1.7820000000000011</c:v>
+                  <c:v>1.0800000000000007</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>1.8020000000000012</c:v>
+                  <c:v>1.0920000000000007</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>1.8220000000000012</c:v>
+                  <c:v>1.1040000000000008</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>1.8420000000000012</c:v>
+                  <c:v>1.1160000000000008</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>1.8620000000000012</c:v>
+                  <c:v>1.1280000000000008</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>1.8820000000000012</c:v>
+                  <c:v>1.1400000000000008</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>1.9020000000000012</c:v>
+                  <c:v>1.1520000000000008</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>1.9220000000000013</c:v>
+                  <c:v>1.1640000000000008</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>1.9420000000000013</c:v>
+                  <c:v>1.1760000000000008</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>1.9620000000000013</c:v>
+                  <c:v>1.1880000000000008</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>1.9820000000000013</c:v>
+                  <c:v>1.2000000000000008</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>2.0020000000000011</c:v>
+                  <c:v>1.2120000000000009</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>2.0220000000000011</c:v>
+                  <c:v>1.2240000000000009</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>2.0420000000000011</c:v>
+                  <c:v>1.2360000000000009</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>2.0620000000000012</c:v>
+                  <c:v>1.2480000000000009</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>2.0820000000000012</c:v>
+                  <c:v>1.2600000000000009</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>2.1020000000000012</c:v>
+                  <c:v>1.2720000000000009</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>2.1220000000000012</c:v>
+                  <c:v>1.2840000000000009</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>2.1420000000000012</c:v>
+                  <c:v>1.2960000000000009</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>2.1620000000000013</c:v>
+                  <c:v>1.3080000000000009</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>2.1820000000000013</c:v>
+                  <c:v>1.320000000000001</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>2.2020000000000013</c:v>
+                  <c:v>1.332000000000001</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>2.2220000000000013</c:v>
+                  <c:v>1.344000000000001</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>2.2420000000000013</c:v>
+                  <c:v>1.356000000000001</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>2.2620000000000013</c:v>
+                  <c:v>1.368000000000001</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>2.2820000000000014</c:v>
+                  <c:v>1.380000000000001</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>2.3020000000000014</c:v>
+                  <c:v>1.392000000000001</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>2.3220000000000014</c:v>
+                  <c:v>1.404000000000001</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>2.3420000000000014</c:v>
+                  <c:v>1.416000000000001</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>2.3620000000000014</c:v>
+                  <c:v>1.428000000000001</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>2.3820000000000014</c:v>
+                  <c:v>1.4400000000000011</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>2.4020000000000015</c:v>
+                  <c:v>1.4520000000000011</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>2.4220000000000015</c:v>
+                  <c:v>1.4640000000000011</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>2.4420000000000015</c:v>
+                  <c:v>1.4760000000000011</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>2.4620000000000015</c:v>
+                  <c:v>1.4880000000000011</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>2.4820000000000015</c:v>
+                  <c:v>1.5000000000000011</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>2.5020000000000016</c:v>
+                  <c:v>1.5120000000000011</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>2.5220000000000016</c:v>
+                  <c:v>1.5240000000000011</c:v>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>2.5420000000000016</c:v>
+                  <c:v>1.5360000000000011</c:v>
                 </c:pt>
                 <c:pt idx="128">
-                  <c:v>2.5620000000000016</c:v>
+                  <c:v>1.5480000000000012</c:v>
                 </c:pt>
                 <c:pt idx="129">
-                  <c:v>2.5820000000000016</c:v>
+                  <c:v>1.5600000000000012</c:v>
                 </c:pt>
                 <c:pt idx="130">
-                  <c:v>2.6020000000000016</c:v>
+                  <c:v>1.5720000000000012</c:v>
                 </c:pt>
                 <c:pt idx="131">
-                  <c:v>2.6220000000000017</c:v>
+                  <c:v>1.5840000000000012</c:v>
                 </c:pt>
                 <c:pt idx="132">
-                  <c:v>2.6420000000000017</c:v>
+                  <c:v>1.5960000000000012</c:v>
                 </c:pt>
                 <c:pt idx="133">
-                  <c:v>2.6620000000000017</c:v>
+                  <c:v>1.6080000000000012</c:v>
                 </c:pt>
                 <c:pt idx="134">
-                  <c:v>2.6820000000000017</c:v>
+                  <c:v>1.6200000000000012</c:v>
                 </c:pt>
                 <c:pt idx="135">
-                  <c:v>2.7020000000000017</c:v>
+                  <c:v>1.6320000000000012</c:v>
                 </c:pt>
                 <c:pt idx="136">
-                  <c:v>2.7220000000000018</c:v>
+                  <c:v>1.6440000000000012</c:v>
                 </c:pt>
                 <c:pt idx="137">
-                  <c:v>2.7420000000000018</c:v>
+                  <c:v>1.6560000000000012</c:v>
                 </c:pt>
                 <c:pt idx="138">
-                  <c:v>2.7620000000000018</c:v>
+                  <c:v>1.6680000000000013</c:v>
                 </c:pt>
                 <c:pt idx="139">
-                  <c:v>2.7820000000000018</c:v>
+                  <c:v>1.6800000000000013</c:v>
                 </c:pt>
                 <c:pt idx="140">
-                  <c:v>2.8020000000000018</c:v>
+                  <c:v>1.6920000000000013</c:v>
                 </c:pt>
                 <c:pt idx="141">
-                  <c:v>2.8220000000000018</c:v>
+                  <c:v>1.7040000000000013</c:v>
                 </c:pt>
                 <c:pt idx="142">
-                  <c:v>2.8420000000000019</c:v>
+                  <c:v>1.7160000000000013</c:v>
                 </c:pt>
                 <c:pt idx="143">
-                  <c:v>2.8620000000000019</c:v>
+                  <c:v>1.7280000000000013</c:v>
                 </c:pt>
                 <c:pt idx="144">
-                  <c:v>2.8820000000000019</c:v>
+                  <c:v>1.7400000000000013</c:v>
                 </c:pt>
                 <c:pt idx="145">
-                  <c:v>2.9020000000000019</c:v>
+                  <c:v>1.7520000000000013</c:v>
                 </c:pt>
                 <c:pt idx="146">
-                  <c:v>2.9220000000000019</c:v>
+                  <c:v>1.7640000000000013</c:v>
                 </c:pt>
                 <c:pt idx="147">
-                  <c:v>2.9420000000000019</c:v>
+                  <c:v>1.7760000000000014</c:v>
                 </c:pt>
                 <c:pt idx="148">
-                  <c:v>2.962000000000002</c:v>
+                  <c:v>1.7880000000000014</c:v>
                 </c:pt>
                 <c:pt idx="149">
-                  <c:v>2.982000000000002</c:v>
+                  <c:v>1.8000000000000014</c:v>
                 </c:pt>
                 <c:pt idx="150">
-                  <c:v>3.002000000000002</c:v>
+                  <c:v>1.8120000000000014</c:v>
                 </c:pt>
                 <c:pt idx="151">
-                  <c:v>3.022000000000002</c:v>
+                  <c:v>1.8240000000000014</c:v>
                 </c:pt>
                 <c:pt idx="152">
-                  <c:v>3.042000000000002</c:v>
+                  <c:v>1.8360000000000014</c:v>
                 </c:pt>
                 <c:pt idx="153">
-                  <c:v>3.0620000000000021</c:v>
+                  <c:v>1.8480000000000014</c:v>
                 </c:pt>
                 <c:pt idx="154">
-                  <c:v>3.0820000000000021</c:v>
+                  <c:v>1.8600000000000014</c:v>
                 </c:pt>
                 <c:pt idx="155">
-                  <c:v>3.1020000000000021</c:v>
+                  <c:v>1.8720000000000014</c:v>
                 </c:pt>
                 <c:pt idx="156">
-                  <c:v>3.1220000000000021</c:v>
+                  <c:v>1.8840000000000015</c:v>
                 </c:pt>
                 <c:pt idx="157">
-                  <c:v>3.1420000000000021</c:v>
+                  <c:v>1.8960000000000015</c:v>
                 </c:pt>
                 <c:pt idx="158">
-                  <c:v>3.1620000000000021</c:v>
+                  <c:v>1.9080000000000015</c:v>
                 </c:pt>
                 <c:pt idx="159">
-                  <c:v>3.1820000000000022</c:v>
+                  <c:v>1.9200000000000015</c:v>
                 </c:pt>
                 <c:pt idx="160">
-                  <c:v>3.2020000000000022</c:v>
+                  <c:v>1.9320000000000015</c:v>
                 </c:pt>
                 <c:pt idx="161">
-                  <c:v>3.2220000000000022</c:v>
+                  <c:v>1.9440000000000015</c:v>
                 </c:pt>
                 <c:pt idx="162">
-                  <c:v>3.2420000000000022</c:v>
+                  <c:v>1.9560000000000015</c:v>
                 </c:pt>
                 <c:pt idx="163">
-                  <c:v>3.2620000000000022</c:v>
+                  <c:v>1.9680000000000015</c:v>
                 </c:pt>
                 <c:pt idx="164">
-                  <c:v>3.2820000000000022</c:v>
+                  <c:v>1.9800000000000015</c:v>
                 </c:pt>
                 <c:pt idx="165">
-                  <c:v>3.3020000000000023</c:v>
+                  <c:v>1.9920000000000015</c:v>
                 </c:pt>
                 <c:pt idx="166">
-                  <c:v>3.3220000000000023</c:v>
+                  <c:v>2.0040000000000013</c:v>
                 </c:pt>
                 <c:pt idx="167">
-                  <c:v>3.3420000000000023</c:v>
+                  <c:v>2.0160000000000013</c:v>
                 </c:pt>
                 <c:pt idx="168">
-                  <c:v>3.3620000000000023</c:v>
+                  <c:v>2.0280000000000014</c:v>
                 </c:pt>
                 <c:pt idx="169">
-                  <c:v>3.3820000000000023</c:v>
+                  <c:v>2.0400000000000014</c:v>
                 </c:pt>
                 <c:pt idx="170">
-                  <c:v>3.4020000000000024</c:v>
+                  <c:v>2.0520000000000014</c:v>
                 </c:pt>
                 <c:pt idx="171">
-                  <c:v>3.4220000000000024</c:v>
+                  <c:v>2.0640000000000014</c:v>
                 </c:pt>
                 <c:pt idx="172">
-                  <c:v>3.4420000000000024</c:v>
+                  <c:v>2.0760000000000014</c:v>
                 </c:pt>
                 <c:pt idx="173">
-                  <c:v>3.4620000000000024</c:v>
+                  <c:v>2.0880000000000014</c:v>
                 </c:pt>
                 <c:pt idx="174">
-                  <c:v>3.4820000000000024</c:v>
+                  <c:v>2.1000000000000014</c:v>
                 </c:pt>
                 <c:pt idx="175">
-                  <c:v>3.5020000000000024</c:v>
+                  <c:v>2.1120000000000014</c:v>
                 </c:pt>
                 <c:pt idx="176">
-                  <c:v>3.5220000000000025</c:v>
+                  <c:v>2.1240000000000014</c:v>
                 </c:pt>
                 <c:pt idx="177">
-                  <c:v>3.5420000000000025</c:v>
+                  <c:v>2.1360000000000015</c:v>
                 </c:pt>
                 <c:pt idx="178">
-                  <c:v>3.5620000000000025</c:v>
+                  <c:v>2.1480000000000015</c:v>
                 </c:pt>
                 <c:pt idx="179">
-                  <c:v>3.5820000000000025</c:v>
+                  <c:v>2.1600000000000015</c:v>
                 </c:pt>
                 <c:pt idx="180">
-                  <c:v>3.6020000000000025</c:v>
+                  <c:v>2.1720000000000015</c:v>
                 </c:pt>
                 <c:pt idx="181">
-                  <c:v>3.6220000000000026</c:v>
+                  <c:v>2.1840000000000015</c:v>
                 </c:pt>
                 <c:pt idx="182">
-                  <c:v>3.6420000000000026</c:v>
-                </c:pt>
-                <c:pt idx="183">
-                  <c:v>3.6620000000000026</c:v>
+                  <c:v>2.1960000000000015</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2064,58 +2074,58 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>1.682000000000001</c:v>
+                  <c:v>1.0200000000000007</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.7020000000000011</c:v>
+                  <c:v>1.0320000000000007</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.7220000000000011</c:v>
+                  <c:v>1.0440000000000007</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.7420000000000011</c:v>
+                  <c:v>1.0560000000000007</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.7620000000000011</c:v>
+                  <c:v>1.0680000000000007</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.7820000000000011</c:v>
+                  <c:v>1.0800000000000007</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.8020000000000012</c:v>
+                  <c:v>1.0920000000000007</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.8220000000000012</c:v>
+                  <c:v>1.1040000000000008</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.8420000000000012</c:v>
+                  <c:v>1.1160000000000008</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.8620000000000012</c:v>
+                  <c:v>1.1280000000000008</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.8820000000000012</c:v>
+                  <c:v>1.1400000000000008</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.9020000000000012</c:v>
+                  <c:v>1.1520000000000008</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.9220000000000013</c:v>
+                  <c:v>1.1640000000000008</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.9420000000000013</c:v>
+                  <c:v>1.1760000000000008</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.9620000000000013</c:v>
+                  <c:v>1.1880000000000008</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.9820000000000013</c:v>
+                  <c:v>1.2000000000000008</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.0020000000000011</c:v>
+                  <c:v>1.2120000000000009</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.0220000000000011</c:v>
+                  <c:v>1.2240000000000009</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2456,67 +2466,67 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2E-3</c:v>
+                  <c:v>1.2E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0000000000000001E-3</c:v>
+                  <c:v>2.4E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.0000000000000001E-3</c:v>
+                  <c:v>3.6000000000000004E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.0000000000000002E-3</c:v>
+                  <c:v>4.8000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.01</c:v>
+                  <c:v>0.06</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.2E-2</c:v>
+                  <c:v>7.1999999999999995E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.4E-2</c:v>
+                  <c:v>8.3999999999999991E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.6E-2</c:v>
+                  <c:v>9.5999999999999988E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.8000000000000002E-2</c:v>
+                  <c:v>0.10799999999999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.0000000000000004E-2</c:v>
+                  <c:v>0.11999999999999998</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.2000000000000006E-2</c:v>
+                  <c:v>0.13199999999999998</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.4000000000000007E-2</c:v>
+                  <c:v>0.14399999999999999</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.6000000000000009E-2</c:v>
+                  <c:v>0.156</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.8000000000000011E-2</c:v>
+                  <c:v>0.16800000000000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.0000000000000013E-2</c:v>
+                  <c:v>0.18000000000000002</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.2000000000000015E-2</c:v>
+                  <c:v>0.19200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3.4000000000000016E-2</c:v>
+                  <c:v>0.20400000000000004</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3.6000000000000018E-2</c:v>
+                  <c:v>0.21600000000000005</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3.800000000000002E-2</c:v>
+                  <c:v>0.22800000000000006</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>4.0000000000000022E-2</c:v>
+                  <c:v>0.24000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>4.2000000000000023E-2</c:v>
+                  <c:v>0.25200000000000006</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2555,10 +2565,16 @@
                   <c:v>7.8878779999999997</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.3554080000000006</c:v>
+                  <c:v>8.5757750000000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>9.2636719999999997</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.2585786666666667</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9.3401083333333332</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>9.9362890000000004</c:v>
@@ -4885,7 +4901,7 @@
   <dimension ref="A1:S185"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="S25" sqref="S25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4910,8 +4926,8 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2">
-        <f>2*10^-3</f>
-        <v>2E-3</v>
+        <f>12*10^-3</f>
+        <v>1.2E-2</v>
       </c>
       <c r="B2">
         <v>0.80015999999999998</v>
@@ -4928,8 +4944,8 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3">
-        <f>A2+20*10^-3</f>
-        <v>2.1999999999999999E-2</v>
+        <f>A2+12*10^-3</f>
+        <v>2.4E-2</v>
       </c>
       <c r="B3">
         <v>0.8044</v>
@@ -4941,8 +4957,8 @@
         <v>1.6203920000000001</v>
       </c>
       <c r="G3">
-        <f>G2+2*10^-3</f>
-        <v>2E-3</v>
+        <f>A2</f>
+        <v>1.2E-2</v>
       </c>
       <c r="H3">
         <f>D86</f>
@@ -4951,8 +4967,8 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4">
-        <f t="shared" ref="A4:A67" si="0">A3+20*10^-3</f>
-        <v>4.1999999999999996E-2</v>
+        <f t="shared" ref="A4:A67" si="0">A3+12*10^-3</f>
+        <v>3.6000000000000004E-2</v>
       </c>
       <c r="B4">
         <v>0.8044</v>
@@ -4964,8 +4980,8 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G4:G23" si="1">G3+2*10^-3</f>
-        <v>4.0000000000000001E-3</v>
+        <f t="shared" ref="G4:G23" si="1">A3</f>
+        <v>2.4E-2</v>
       </c>
       <c r="H4">
         <f t="shared" ref="H4:H23" si="2">D87</f>
@@ -4975,7 +4991,7 @@
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5">
         <f t="shared" si="0"/>
-        <v>6.2E-2</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="B5">
         <v>0.80432000000000003</v>
@@ -4988,7 +5004,7 @@
       </c>
       <c r="G5">
         <f t="shared" si="1"/>
-        <v>6.0000000000000001E-3</v>
+        <v>3.6000000000000004E-2</v>
       </c>
       <c r="H5">
         <f t="shared" si="2"/>
@@ -4998,7 +5014,7 @@
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6">
         <f t="shared" si="0"/>
-        <v>8.2000000000000003E-2</v>
+        <v>0.06</v>
       </c>
       <c r="B6">
         <v>0.8044</v>
@@ -5011,7 +5027,7 @@
       </c>
       <c r="G6">
         <f t="shared" si="1"/>
-        <v>8.0000000000000002E-3</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="H6">
         <f t="shared" si="2"/>
@@ -5021,7 +5037,7 @@
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7">
         <f t="shared" si="0"/>
-        <v>0.10200000000000001</v>
+        <v>7.1999999999999995E-2</v>
       </c>
       <c r="B7">
         <v>0.80432000000000003</v>
@@ -5034,7 +5050,7 @@
       </c>
       <c r="G7">
         <f t="shared" si="1"/>
-        <v>0.01</v>
+        <v>0.06</v>
       </c>
       <c r="H7">
         <f t="shared" si="2"/>
@@ -5044,7 +5060,7 @@
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8">
         <f t="shared" si="0"/>
-        <v>0.12200000000000001</v>
+        <v>8.3999999999999991E-2</v>
       </c>
       <c r="B8">
         <v>0.8044</v>
@@ -5057,7 +5073,7 @@
       </c>
       <c r="G8">
         <f t="shared" si="1"/>
-        <v>1.2E-2</v>
+        <v>7.1999999999999995E-2</v>
       </c>
       <c r="H8">
         <f t="shared" si="2"/>
@@ -5067,7 +5083,7 @@
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9">
         <f t="shared" si="0"/>
-        <v>0.14200000000000002</v>
+        <v>9.5999999999999988E-2</v>
       </c>
       <c r="B9">
         <v>0.8044</v>
@@ -5080,7 +5096,7 @@
       </c>
       <c r="G9">
         <f t="shared" si="1"/>
-        <v>1.4E-2</v>
+        <v>8.3999999999999991E-2</v>
       </c>
       <c r="H9">
         <f t="shared" si="2"/>
@@ -5090,7 +5106,7 @@
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10">
         <f t="shared" si="0"/>
-        <v>0.16200000000000001</v>
+        <v>0.10799999999999998</v>
       </c>
       <c r="B10">
         <v>0.8044</v>
@@ -5103,7 +5119,7 @@
       </c>
       <c r="G10">
         <f t="shared" si="1"/>
-        <v>1.6E-2</v>
+        <v>9.5999999999999988E-2</v>
       </c>
       <c r="H10">
         <f t="shared" si="2"/>
@@ -5113,7 +5129,7 @@
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11">
         <f t="shared" si="0"/>
-        <v>0.182</v>
+        <v>0.11999999999999998</v>
       </c>
       <c r="B11">
         <v>0.80432000000000003</v>
@@ -5126,17 +5142,17 @@
       </c>
       <c r="G11">
         <f t="shared" si="1"/>
-        <v>1.8000000000000002E-2</v>
+        <v>0.10799999999999998</v>
       </c>
       <c r="H11">
-        <f t="shared" si="2"/>
-        <v>9.3554080000000006</v>
+        <f>(H10+H12)/2</f>
+        <v>8.5757750000000001</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12">
         <f t="shared" si="0"/>
-        <v>0.20199999999999999</v>
+        <v>0.13199999999999998</v>
       </c>
       <c r="B12">
         <v>0.8044</v>
@@ -5149,7 +5165,7 @@
       </c>
       <c r="G12">
         <f t="shared" si="1"/>
-        <v>2.0000000000000004E-2</v>
+        <v>0.11999999999999998</v>
       </c>
       <c r="H12">
         <f t="shared" si="2"/>
@@ -5159,7 +5175,7 @@
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13">
         <f t="shared" si="0"/>
-        <v>0.22199999999999998</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="B13">
         <v>0.8044</v>
@@ -5172,13 +5188,17 @@
       </c>
       <c r="G13">
         <f t="shared" si="1"/>
-        <v>2.2000000000000006E-2</v>
+        <v>0.13199999999999998</v>
+      </c>
+      <c r="H13">
+        <f>(H12+H11+H15)/3</f>
+        <v>9.2585786666666667</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14">
         <f t="shared" si="0"/>
-        <v>0.24199999999999997</v>
+        <v>0.156</v>
       </c>
       <c r="B14">
         <v>0.80432000000000003</v>
@@ -5191,13 +5211,17 @@
       </c>
       <c r="G14">
         <f t="shared" si="1"/>
-        <v>2.4000000000000007E-2</v>
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="H14">
+        <f>(H11+H12+H16)/3</f>
+        <v>9.3401083333333332</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15">
         <f t="shared" si="0"/>
-        <v>0.26199999999999996</v>
+        <v>0.16800000000000001</v>
       </c>
       <c r="B15">
         <v>0.80432000000000003</v>
@@ -5210,7 +5234,7 @@
       </c>
       <c r="G15">
         <f t="shared" si="1"/>
-        <v>2.6000000000000009E-2</v>
+        <v>0.156</v>
       </c>
       <c r="H15">
         <f t="shared" si="2"/>
@@ -5220,7 +5244,7 @@
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16">
         <f t="shared" si="0"/>
-        <v>0.28199999999999997</v>
+        <v>0.18000000000000002</v>
       </c>
       <c r="B16">
         <v>0.80432000000000003</v>
@@ -5233,7 +5257,7 @@
       </c>
       <c r="G16">
         <f t="shared" si="1"/>
-        <v>2.8000000000000011E-2</v>
+        <v>0.16800000000000001</v>
       </c>
       <c r="H16">
         <f t="shared" si="2"/>
@@ -5243,7 +5267,7 @@
     <row r="17" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A17">
         <f t="shared" si="0"/>
-        <v>0.30199999999999999</v>
+        <v>0.19200000000000003</v>
       </c>
       <c r="B17">
         <v>0.8044</v>
@@ -5256,7 +5280,7 @@
       </c>
       <c r="G17">
         <f t="shared" si="1"/>
-        <v>3.0000000000000013E-2</v>
+        <v>0.18000000000000002</v>
       </c>
       <c r="H17">
         <f t="shared" si="2"/>
@@ -5266,7 +5290,7 @@
     <row r="18" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A18">
         <f t="shared" si="0"/>
-        <v>0.32200000000000001</v>
+        <v>0.20400000000000004</v>
       </c>
       <c r="B18">
         <v>0.80432000000000003</v>
@@ -5279,7 +5303,7 @@
       </c>
       <c r="G18">
         <f t="shared" si="1"/>
-        <v>3.2000000000000015E-2</v>
+        <v>0.19200000000000003</v>
       </c>
       <c r="H18">
         <f t="shared" si="2"/>
@@ -5289,7 +5313,7 @@
     <row r="19" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A19">
         <f t="shared" si="0"/>
-        <v>0.34200000000000003</v>
+        <v>0.21600000000000005</v>
       </c>
       <c r="B19">
         <v>0.8044</v>
@@ -5302,7 +5326,7 @@
       </c>
       <c r="G19">
         <f t="shared" si="1"/>
-        <v>3.4000000000000016E-2</v>
+        <v>0.20400000000000004</v>
       </c>
       <c r="H19">
         <f t="shared" si="2"/>
@@ -5312,7 +5336,7 @@
     <row r="20" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A20">
         <f t="shared" si="0"/>
-        <v>0.36200000000000004</v>
+        <v>0.22800000000000006</v>
       </c>
       <c r="B20">
         <v>0.8044</v>
@@ -5325,7 +5349,7 @@
       </c>
       <c r="G20">
         <f t="shared" si="1"/>
-        <v>3.6000000000000018E-2</v>
+        <v>0.21600000000000005</v>
       </c>
       <c r="H20">
         <f t="shared" si="2"/>
@@ -5335,7 +5359,7 @@
     <row r="21" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A21">
         <f t="shared" si="0"/>
-        <v>0.38200000000000006</v>
+        <v>0.24000000000000007</v>
       </c>
       <c r="B21">
         <v>0.8044</v>
@@ -5348,7 +5372,7 @@
       </c>
       <c r="G21">
         <f t="shared" si="1"/>
-        <v>3.800000000000002E-2</v>
+        <v>0.22800000000000006</v>
       </c>
       <c r="H21">
         <f t="shared" si="2"/>
@@ -5358,7 +5382,7 @@
     <row r="22" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A22">
         <f t="shared" si="0"/>
-        <v>0.40200000000000008</v>
+        <v>0.25200000000000006</v>
       </c>
       <c r="B22">
         <v>0.8044</v>
@@ -5371,7 +5395,7 @@
       </c>
       <c r="G22">
         <f t="shared" si="1"/>
-        <v>4.0000000000000022E-2</v>
+        <v>0.24000000000000007</v>
       </c>
       <c r="H22">
         <f t="shared" si="2"/>
@@ -5387,7 +5411,7 @@
     <row r="23" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A23">
         <f t="shared" si="0"/>
-        <v>0.4220000000000001</v>
+        <v>0.26400000000000007</v>
       </c>
       <c r="B23">
         <v>0.80432000000000003</v>
@@ -5400,7 +5424,7 @@
       </c>
       <c r="G23">
         <f t="shared" si="1"/>
-        <v>4.2000000000000023E-2</v>
+        <v>0.25200000000000006</v>
       </c>
       <c r="H23">
         <f t="shared" si="2"/>
@@ -5417,7 +5441,7 @@
     <row r="24" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A24">
         <f t="shared" si="0"/>
-        <v>0.44200000000000012</v>
+        <v>0.27600000000000008</v>
       </c>
       <c r="B24">
         <v>0.8044</v>
@@ -5432,7 +5456,7 @@
     <row r="25" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A25">
         <f t="shared" si="0"/>
-        <v>0.46200000000000013</v>
+        <v>0.28800000000000009</v>
       </c>
       <c r="B25">
         <v>0.80432000000000003</v>
@@ -5447,13 +5471,14 @@
         <v>4</v>
       </c>
       <c r="S25" s="1">
-        <v>1.2500000000000001E-2</v>
+        <f>(G8-4*10^-3+G9)/2</f>
+        <v>7.5999999999999984E-2</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A26">
         <f t="shared" si="0"/>
-        <v>0.48200000000000015</v>
+        <v>0.3000000000000001</v>
       </c>
       <c r="B26">
         <v>0.8044</v>
@@ -5468,7 +5493,7 @@
     <row r="27" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A27">
         <f t="shared" si="0"/>
-        <v>0.50200000000000011</v>
+        <v>0.31200000000000011</v>
       </c>
       <c r="B27">
         <v>0.80432000000000003</v>
@@ -5483,7 +5508,7 @@
     <row r="28" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A28">
         <f t="shared" si="0"/>
-        <v>0.52200000000000013</v>
+        <v>0.32400000000000012</v>
       </c>
       <c r="B28">
         <v>0.8044</v>
@@ -5504,7 +5529,7 @@
     <row r="29" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A29">
         <f t="shared" si="0"/>
-        <v>0.54200000000000015</v>
+        <v>0.33600000000000013</v>
       </c>
       <c r="B29">
         <v>0.8044</v>
@@ -5525,7 +5550,7 @@
     <row r="30" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A30">
         <f t="shared" si="0"/>
-        <v>0.56200000000000017</v>
+        <v>0.34800000000000014</v>
       </c>
       <c r="B30">
         <v>0.8044</v>
@@ -5546,7 +5571,7 @@
     <row r="31" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A31">
         <f t="shared" si="0"/>
-        <v>0.58200000000000018</v>
+        <v>0.36000000000000015</v>
       </c>
       <c r="B31">
         <v>0.8044</v>
@@ -5567,7 +5592,7 @@
     <row r="32" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A32">
         <f t="shared" si="0"/>
-        <v>0.6020000000000002</v>
+        <v>0.37200000000000016</v>
       </c>
       <c r="B32">
         <v>0.8044</v>
@@ -5582,7 +5607,7 @@
     <row r="33" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A33">
         <f t="shared" si="0"/>
-        <v>0.62200000000000022</v>
+        <v>0.38400000000000017</v>
       </c>
       <c r="B33">
         <v>0.80432000000000003</v>
@@ -5598,13 +5623,13 @@
       </c>
       <c r="S33">
         <f>(S25*(S31*S30+S29*S28))/(S31)</f>
-        <v>3.7473214285714289E-3</v>
+        <v>2.2783714285714282E-2</v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A34">
         <f t="shared" si="0"/>
-        <v>0.64200000000000024</v>
+        <v>0.39600000000000019</v>
       </c>
       <c r="B34">
         <v>0.8044</v>
@@ -5619,7 +5644,7 @@
     <row r="35" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A35">
         <f t="shared" si="0"/>
-        <v>0.66200000000000025</v>
+        <v>0.4080000000000002</v>
       </c>
       <c r="B35">
         <v>0.8044</v>
@@ -5634,7 +5659,7 @@
     <row r="36" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A36">
         <f t="shared" si="0"/>
-        <v>0.68200000000000027</v>
+        <v>0.42000000000000021</v>
       </c>
       <c r="B36">
         <v>0.80432000000000003</v>
@@ -5649,7 +5674,7 @@
     <row r="37" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A37">
         <f t="shared" si="0"/>
-        <v>0.70200000000000029</v>
+        <v>0.43200000000000022</v>
       </c>
       <c r="B37">
         <v>0.8044</v>
@@ -5664,7 +5689,7 @@
     <row r="38" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A38">
         <f t="shared" si="0"/>
-        <v>0.72200000000000031</v>
+        <v>0.44400000000000023</v>
       </c>
       <c r="B38">
         <v>0.8044</v>
@@ -5679,7 +5704,7 @@
     <row r="39" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A39">
         <f t="shared" si="0"/>
-        <v>0.74200000000000033</v>
+        <v>0.45600000000000024</v>
       </c>
       <c r="B39">
         <v>0.80432000000000003</v>
@@ -5694,7 +5719,7 @@
     <row r="40" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A40">
         <f t="shared" si="0"/>
-        <v>0.76200000000000034</v>
+        <v>0.46800000000000025</v>
       </c>
       <c r="B40">
         <v>0.80432000000000003</v>
@@ -5709,7 +5734,7 @@
     <row r="41" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A41">
         <f t="shared" si="0"/>
-        <v>0.78200000000000036</v>
+        <v>0.48000000000000026</v>
       </c>
       <c r="B41">
         <v>0.80432000000000003</v>
@@ -5724,7 +5749,7 @@
     <row r="42" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A42">
         <f t="shared" si="0"/>
-        <v>0.80200000000000038</v>
+        <v>0.49200000000000027</v>
       </c>
       <c r="B42">
         <v>0.80376000000000003</v>
@@ -5739,7 +5764,7 @@
     <row r="43" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A43">
         <f t="shared" si="0"/>
-        <v>0.8220000000000004</v>
+        <v>0.50400000000000023</v>
       </c>
       <c r="B43">
         <v>0.8044</v>
@@ -5754,7 +5779,7 @@
     <row r="44" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A44">
         <f t="shared" si="0"/>
-        <v>0.84200000000000041</v>
+        <v>0.51600000000000024</v>
       </c>
       <c r="B44">
         <v>0.8044</v>
@@ -5769,7 +5794,7 @@
     <row r="45" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A45">
         <f t="shared" si="0"/>
-        <v>0.86200000000000043</v>
+        <v>0.52800000000000025</v>
       </c>
       <c r="B45">
         <v>0.80391999999999997</v>
@@ -5784,7 +5809,7 @@
     <row r="46" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A46">
         <f t="shared" si="0"/>
-        <v>0.88200000000000045</v>
+        <v>0.54000000000000026</v>
       </c>
       <c r="B46">
         <v>0.8044</v>
@@ -5799,7 +5824,7 @@
     <row r="47" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A47">
         <f t="shared" si="0"/>
-        <v>0.90200000000000047</v>
+        <v>0.55200000000000027</v>
       </c>
       <c r="B47">
         <v>0.80408000000000002</v>
@@ -5814,7 +5839,7 @@
     <row r="48" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A48">
         <f t="shared" si="0"/>
-        <v>0.92200000000000049</v>
+        <v>0.56400000000000028</v>
       </c>
       <c r="B48">
         <v>0.80423999999999995</v>
@@ -5829,7 +5854,7 @@
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49">
         <f t="shared" si="0"/>
-        <v>0.9420000000000005</v>
+        <v>0.57600000000000029</v>
       </c>
       <c r="B49">
         <v>0.80432000000000003</v>
@@ -5844,7 +5869,7 @@
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50">
         <f t="shared" si="0"/>
-        <v>0.96200000000000052</v>
+        <v>0.5880000000000003</v>
       </c>
       <c r="B50">
         <v>0.80432000000000003</v>
@@ -5859,7 +5884,7 @@
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51">
         <f t="shared" si="0"/>
-        <v>0.98200000000000054</v>
+        <v>0.60000000000000031</v>
       </c>
       <c r="B51">
         <v>0.80415999999999999</v>
@@ -5874,7 +5899,7 @@
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52">
         <f t="shared" si="0"/>
-        <v>1.0020000000000004</v>
+        <v>0.61200000000000032</v>
       </c>
       <c r="B52">
         <v>0.8044</v>
@@ -5889,7 +5914,7 @@
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53">
         <f t="shared" si="0"/>
-        <v>1.0220000000000005</v>
+        <v>0.62400000000000033</v>
       </c>
       <c r="B53">
         <v>0.80423999999999995</v>
@@ -5904,7 +5929,7 @@
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54">
         <f t="shared" si="0"/>
-        <v>1.0420000000000005</v>
+        <v>0.63600000000000034</v>
       </c>
       <c r="B54">
         <v>0.80432000000000003</v>
@@ -5919,7 +5944,7 @@
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55">
         <f t="shared" si="0"/>
-        <v>1.0620000000000005</v>
+        <v>0.64800000000000035</v>
       </c>
       <c r="B55">
         <v>0.8044</v>
@@ -5934,7 +5959,7 @@
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56">
         <f t="shared" si="0"/>
-        <v>1.0820000000000005</v>
+        <v>0.66000000000000036</v>
       </c>
       <c r="B56">
         <v>0.80408000000000002</v>
@@ -5949,7 +5974,7 @@
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57">
         <f t="shared" si="0"/>
-        <v>1.1020000000000005</v>
+        <v>0.67200000000000037</v>
       </c>
       <c r="B57">
         <v>0.8044</v>
@@ -5964,7 +5989,7 @@
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58">
         <f t="shared" si="0"/>
-        <v>1.1220000000000006</v>
+        <v>0.68400000000000039</v>
       </c>
       <c r="B58">
         <v>0.80432000000000003</v>
@@ -5979,7 +6004,7 @@
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59">
         <f t="shared" si="0"/>
-        <v>1.1420000000000006</v>
+        <v>0.6960000000000004</v>
       </c>
       <c r="B59">
         <v>0.80432000000000003</v>
@@ -5994,7 +6019,7 @@
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60">
         <f t="shared" si="0"/>
-        <v>1.1620000000000006</v>
+        <v>0.70800000000000041</v>
       </c>
       <c r="B60">
         <v>0.8044</v>
@@ -6009,7 +6034,7 @@
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61">
         <f t="shared" si="0"/>
-        <v>1.1820000000000006</v>
+        <v>0.72000000000000042</v>
       </c>
       <c r="B61">
         <v>0.80432000000000003</v>
@@ -6024,7 +6049,7 @@
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62">
         <f t="shared" si="0"/>
-        <v>1.2020000000000006</v>
+        <v>0.73200000000000043</v>
       </c>
       <c r="B62">
         <v>0.80432000000000003</v>
@@ -6039,7 +6064,7 @@
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63">
         <f t="shared" si="0"/>
-        <v>1.2220000000000006</v>
+        <v>0.74400000000000044</v>
       </c>
       <c r="B63">
         <v>0.8044</v>
@@ -6054,7 +6079,7 @@
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64">
         <f t="shared" si="0"/>
-        <v>1.2420000000000007</v>
+        <v>0.75600000000000045</v>
       </c>
       <c r="B64">
         <v>0.80423999999999995</v>
@@ -6069,7 +6094,7 @@
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65">
         <f t="shared" si="0"/>
-        <v>1.2620000000000007</v>
+        <v>0.76800000000000046</v>
       </c>
       <c r="B65">
         <v>0.8044</v>
@@ -6084,7 +6109,7 @@
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66">
         <f t="shared" si="0"/>
-        <v>1.2820000000000007</v>
+        <v>0.78000000000000047</v>
       </c>
       <c r="B66">
         <v>0.80432000000000003</v>
@@ -6099,7 +6124,7 @@
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67">
         <f t="shared" si="0"/>
-        <v>1.3020000000000007</v>
+        <v>0.79200000000000048</v>
       </c>
       <c r="B67">
         <v>0.8044</v>
@@ -6113,8 +6138,8 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68">
-        <f t="shared" ref="A68:A131" si="3">A67+20*10^-3</f>
-        <v>1.3220000000000007</v>
+        <f t="shared" ref="A68:A131" si="3">A67+12*10^-3</f>
+        <v>0.80400000000000049</v>
       </c>
       <c r="B68">
         <v>0.80432000000000003</v>
@@ -6129,7 +6154,7 @@
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69">
         <f t="shared" si="3"/>
-        <v>1.3420000000000007</v>
+        <v>0.8160000000000005</v>
       </c>
       <c r="B69">
         <v>0.8044</v>
@@ -6144,7 +6169,7 @@
     <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70">
         <f t="shared" si="3"/>
-        <v>1.3620000000000008</v>
+        <v>0.82800000000000051</v>
       </c>
       <c r="B70">
         <v>0.8044</v>
@@ -6159,7 +6184,7 @@
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71">
         <f t="shared" si="3"/>
-        <v>1.3820000000000008</v>
+        <v>0.84000000000000052</v>
       </c>
       <c r="B71">
         <v>0.8044</v>
@@ -6174,7 +6199,7 @@
     <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72">
         <f t="shared" si="3"/>
-        <v>1.4020000000000008</v>
+        <v>0.85200000000000053</v>
       </c>
       <c r="B72">
         <v>0.80432000000000003</v>
@@ -6189,7 +6214,7 @@
     <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73">
         <f t="shared" si="3"/>
-        <v>1.4220000000000008</v>
+        <v>0.86400000000000055</v>
       </c>
       <c r="B73">
         <v>0.8044</v>
@@ -6204,7 +6229,7 @@
     <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74">
         <f t="shared" si="3"/>
-        <v>1.4420000000000008</v>
+        <v>0.87600000000000056</v>
       </c>
       <c r="B74">
         <v>0.8044</v>
@@ -6219,7 +6244,7 @@
     <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75">
         <f t="shared" si="3"/>
-        <v>1.4620000000000009</v>
+        <v>0.88800000000000057</v>
       </c>
       <c r="B75">
         <v>0.8044</v>
@@ -6234,7 +6259,7 @@
     <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76">
         <f t="shared" si="3"/>
-        <v>1.4820000000000009</v>
+        <v>0.90000000000000058</v>
       </c>
       <c r="B76">
         <v>0.80344000000000004</v>
@@ -6249,7 +6274,7 @@
     <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77">
         <f t="shared" si="3"/>
-        <v>1.5020000000000009</v>
+        <v>0.91200000000000059</v>
       </c>
       <c r="B77">
         <v>0.80415999999999999</v>
@@ -6264,7 +6289,7 @@
     <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78">
         <f t="shared" si="3"/>
-        <v>1.5220000000000009</v>
+        <v>0.9240000000000006</v>
       </c>
       <c r="B78">
         <v>0.80384</v>
@@ -6279,7 +6304,7 @@
     <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79">
         <f t="shared" si="3"/>
-        <v>1.5420000000000009</v>
+        <v>0.93600000000000061</v>
       </c>
       <c r="B79">
         <v>0.80423999999999995</v>
@@ -6294,7 +6319,7 @@
     <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80">
         <f t="shared" si="3"/>
-        <v>1.5620000000000009</v>
+        <v>0.94800000000000062</v>
       </c>
       <c r="B80">
         <v>0.80408000000000002</v>
@@ -6309,7 +6334,7 @@
     <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81">
         <f t="shared" si="3"/>
-        <v>1.582000000000001</v>
+        <v>0.96000000000000063</v>
       </c>
       <c r="B81">
         <v>0.80432000000000003</v>
@@ -6324,7 +6349,7 @@
     <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82">
         <f t="shared" si="3"/>
-        <v>1.602000000000001</v>
+        <v>0.97200000000000064</v>
       </c>
       <c r="B82">
         <v>0.80432000000000003</v>
@@ -6339,7 +6364,7 @@
     <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83">
         <f t="shared" si="3"/>
-        <v>1.622000000000001</v>
+        <v>0.98400000000000065</v>
       </c>
       <c r="B83">
         <v>0.80384</v>
@@ -6354,7 +6379,7 @@
     <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84">
         <f t="shared" si="3"/>
-        <v>1.642000000000001</v>
+        <v>0.99600000000000066</v>
       </c>
       <c r="B84">
         <v>0.80432000000000003</v>
@@ -6369,7 +6394,7 @@
     <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85">
         <f t="shared" si="3"/>
-        <v>1.662000000000001</v>
+        <v>1.0080000000000007</v>
       </c>
       <c r="B85">
         <v>0.80359999999999998</v>
@@ -6384,7 +6409,7 @@
     <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86">
         <f t="shared" si="3"/>
-        <v>1.682000000000001</v>
+        <v>1.0200000000000007</v>
       </c>
       <c r="B86">
         <v>0.80456000000000005</v>
@@ -6399,7 +6424,7 @@
     <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87">
         <f t="shared" si="3"/>
-        <v>1.7020000000000011</v>
+        <v>1.0320000000000007</v>
       </c>
       <c r="B87">
         <v>0.81072</v>
@@ -6414,7 +6439,7 @@
     <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88">
         <f t="shared" si="3"/>
-        <v>1.7220000000000011</v>
+        <v>1.0440000000000007</v>
       </c>
       <c r="B88">
         <v>0.81911999999999996</v>
@@ -6429,7 +6454,7 @@
     <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89">
         <f t="shared" si="3"/>
-        <v>1.7420000000000011</v>
+        <v>1.0560000000000007</v>
       </c>
       <c r="B89">
         <v>0.83087999999999995</v>
@@ -6444,7 +6469,7 @@
     <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90">
         <f t="shared" si="3"/>
-        <v>1.7620000000000011</v>
+        <v>1.0680000000000007</v>
       </c>
       <c r="B90">
         <v>0.84528000000000003</v>
@@ -6459,7 +6484,7 @@
     <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91">
         <f t="shared" si="3"/>
-        <v>1.7820000000000011</v>
+        <v>1.0800000000000007</v>
       </c>
       <c r="B91">
         <v>0.86136000000000001</v>
@@ -6474,7 +6499,7 @@
     <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92">
         <f t="shared" si="3"/>
-        <v>1.8020000000000012</v>
+        <v>1.0920000000000007</v>
       </c>
       <c r="B92">
         <v>0.88</v>
@@ -6489,7 +6514,7 @@
     <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93">
         <f t="shared" si="3"/>
-        <v>1.8220000000000012</v>
+        <v>1.1040000000000008</v>
       </c>
       <c r="B93">
         <v>0.90064</v>
@@ -6504,7 +6529,7 @@
     <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94">
         <f t="shared" si="3"/>
-        <v>1.8420000000000012</v>
+        <v>1.1160000000000008</v>
       </c>
       <c r="B94">
         <v>0.92512000000000005</v>
@@ -6519,7 +6544,7 @@
     <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95">
         <f t="shared" si="3"/>
-        <v>1.8620000000000012</v>
+        <v>1.1280000000000008</v>
       </c>
       <c r="B95">
         <v>0.94935999999999998</v>
@@ -6534,7 +6559,7 @@
     <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96">
         <f t="shared" si="3"/>
-        <v>1.8820000000000012</v>
+        <v>1.1400000000000008</v>
       </c>
       <c r="B96">
         <v>0.45839999999999997</v>
@@ -6546,7 +6571,7 @@
     <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97">
         <f t="shared" si="3"/>
-        <v>1.9020000000000012</v>
+        <v>1.1520000000000008</v>
       </c>
       <c r="B97">
         <v>5.9279999999999999E-2</v>
@@ -6558,7 +6583,7 @@
     <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98">
         <f t="shared" si="3"/>
-        <v>1.9220000000000013</v>
+        <v>1.1640000000000008</v>
       </c>
       <c r="B98">
         <v>8.5279999999999995E-2</v>
@@ -6573,7 +6598,7 @@
     <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99">
         <f t="shared" si="3"/>
-        <v>1.9420000000000013</v>
+        <v>1.1760000000000008</v>
       </c>
       <c r="B99">
         <v>0.11192000000000001</v>
@@ -6588,7 +6613,7 @@
     <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100">
         <f t="shared" si="3"/>
-        <v>1.9620000000000013</v>
+        <v>1.1880000000000008</v>
       </c>
       <c r="B100">
         <v>0.13832</v>
@@ -6603,7 +6628,7 @@
     <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101">
         <f t="shared" si="3"/>
-        <v>1.9820000000000013</v>
+        <v>1.2000000000000008</v>
       </c>
       <c r="B101">
         <v>0.16528000000000001</v>
@@ -6618,7 +6643,7 @@
     <row r="102" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A102">
         <f t="shared" si="3"/>
-        <v>2.0020000000000011</v>
+        <v>1.2120000000000009</v>
       </c>
       <c r="B102">
         <v>0.19231999999999999</v>
@@ -6633,7 +6658,7 @@
     <row r="103" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A103">
         <f t="shared" si="3"/>
-        <v>2.0220000000000011</v>
+        <v>1.2240000000000009</v>
       </c>
       <c r="B103">
         <v>0.21984000000000001</v>
@@ -6648,7 +6673,7 @@
     <row r="104" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A104">
         <f t="shared" si="3"/>
-        <v>2.0420000000000011</v>
+        <v>1.2360000000000009</v>
       </c>
       <c r="B104">
         <v>0.24712000000000001</v>
@@ -6663,7 +6688,7 @@
     <row r="105" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A105">
         <f t="shared" si="3"/>
-        <v>2.0620000000000012</v>
+        <v>1.2480000000000009</v>
       </c>
       <c r="B105">
         <v>0.27448</v>
@@ -6678,7 +6703,7 @@
     <row r="106" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A106">
         <f t="shared" si="3"/>
-        <v>2.0820000000000012</v>
+        <v>1.2600000000000009</v>
       </c>
       <c r="B106">
         <v>0.30152000000000001</v>
@@ -6693,7 +6718,7 @@
     <row r="107" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A107">
         <f t="shared" si="3"/>
-        <v>2.1020000000000012</v>
+        <v>1.2720000000000009</v>
       </c>
       <c r="B107">
         <v>0.32872000000000001</v>
@@ -6708,7 +6733,7 @@
     <row r="108" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A108">
         <f t="shared" si="3"/>
-        <v>2.1220000000000012</v>
+        <v>1.2840000000000009</v>
       </c>
       <c r="B108">
         <v>0.35632000000000003</v>
@@ -6723,7 +6748,7 @@
     <row r="109" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A109">
         <f t="shared" si="3"/>
-        <v>2.1420000000000012</v>
+        <v>1.2960000000000009</v>
       </c>
       <c r="B109">
         <v>0.38303999999999999</v>
@@ -6738,7 +6763,7 @@
     <row r="110" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A110">
         <f t="shared" si="3"/>
-        <v>2.1620000000000013</v>
+        <v>1.3080000000000009</v>
       </c>
       <c r="B110">
         <v>0.40976000000000001</v>
@@ -6753,7 +6778,7 @@
     <row r="111" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A111">
         <f t="shared" si="3"/>
-        <v>2.1820000000000013</v>
+        <v>1.320000000000001</v>
       </c>
       <c r="B111">
         <v>0.43680000000000002</v>
@@ -6768,7 +6793,7 @@
     <row r="112" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A112">
         <f t="shared" si="3"/>
-        <v>2.2020000000000013</v>
+        <v>1.332000000000001</v>
       </c>
       <c r="B112">
         <v>0.46392</v>
@@ -6783,7 +6808,7 @@
     <row r="113" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A113">
         <f t="shared" si="3"/>
-        <v>2.2220000000000013</v>
+        <v>1.344000000000001</v>
       </c>
       <c r="B113">
         <v>0.49096000000000001</v>
@@ -6798,7 +6823,7 @@
     <row r="114" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A114">
         <f t="shared" si="3"/>
-        <v>2.2420000000000013</v>
+        <v>1.356000000000001</v>
       </c>
       <c r="B114">
         <v>0.51807999999999998</v>
@@ -6813,7 +6838,7 @@
     <row r="115" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A115">
         <f t="shared" si="3"/>
-        <v>2.2620000000000013</v>
+        <v>1.368000000000001</v>
       </c>
       <c r="B115">
         <v>0.54488000000000003</v>
@@ -6828,7 +6853,7 @@
     <row r="116" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A116">
         <f t="shared" si="3"/>
-        <v>2.2820000000000014</v>
+        <v>1.380000000000001</v>
       </c>
       <c r="B116">
         <v>0.57184000000000001</v>
@@ -6843,7 +6868,7 @@
     <row r="117" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A117">
         <f t="shared" si="3"/>
-        <v>2.3020000000000014</v>
+        <v>1.392000000000001</v>
       </c>
       <c r="B117">
         <v>0.59863999999999995</v>
@@ -6858,7 +6883,7 @@
     <row r="118" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A118">
         <f t="shared" si="3"/>
-        <v>2.3220000000000014</v>
+        <v>1.404000000000001</v>
       </c>
       <c r="B118">
         <v>0.62624000000000002</v>
@@ -6873,7 +6898,7 @@
     <row r="119" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A119">
         <f t="shared" si="3"/>
-        <v>2.3420000000000014</v>
+        <v>1.416000000000001</v>
       </c>
       <c r="B119">
         <v>0.65351999999999999</v>
@@ -6888,7 +6913,7 @@
     <row r="120" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A120">
         <f t="shared" si="3"/>
-        <v>2.3620000000000014</v>
+        <v>1.428000000000001</v>
       </c>
       <c r="B120">
         <v>0.68071999999999999</v>
@@ -6903,7 +6928,7 @@
     <row r="121" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A121">
         <f t="shared" si="3"/>
-        <v>2.3820000000000014</v>
+        <v>1.4400000000000011</v>
       </c>
       <c r="B121">
         <v>0.70791999999999999</v>
@@ -6918,7 +6943,7 @@
     <row r="122" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A122">
         <f t="shared" si="3"/>
-        <v>2.4020000000000015</v>
+        <v>1.4520000000000011</v>
       </c>
       <c r="B122">
         <v>0.73512</v>
@@ -6933,7 +6958,7 @@
     <row r="123" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A123">
         <f t="shared" si="3"/>
-        <v>2.4220000000000015</v>
+        <v>1.4640000000000011</v>
       </c>
       <c r="B123">
         <v>0.76232</v>
@@ -6948,7 +6973,7 @@
     <row r="124" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A124">
         <f t="shared" si="3"/>
-        <v>2.4420000000000015</v>
+        <v>1.4760000000000011</v>
       </c>
       <c r="B124">
         <v>0.78920000000000001</v>
@@ -6963,7 +6988,7 @@
     <row r="125" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A125">
         <f t="shared" si="3"/>
-        <v>2.4620000000000015</v>
+        <v>1.4880000000000011</v>
       </c>
       <c r="B125">
         <v>0.81872</v>
@@ -6978,7 +7003,7 @@
     <row r="126" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A126">
         <f t="shared" si="3"/>
-        <v>2.4820000000000015</v>
+        <v>1.5000000000000011</v>
       </c>
       <c r="B126">
         <v>0.84543999999999997</v>
@@ -6993,7 +7018,7 @@
     <row r="127" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A127">
         <f t="shared" si="3"/>
-        <v>2.5020000000000016</v>
+        <v>1.5120000000000011</v>
       </c>
       <c r="B127">
         <v>0.87256</v>
@@ -7008,7 +7033,7 @@
     <row r="128" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A128">
         <f t="shared" si="3"/>
-        <v>2.5220000000000016</v>
+        <v>1.5240000000000011</v>
       </c>
       <c r="B128">
         <v>0.89951999999999999</v>
@@ -7023,7 +7048,7 @@
     <row r="129" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A129">
         <f t="shared" si="3"/>
-        <v>2.5420000000000016</v>
+        <v>1.5360000000000011</v>
       </c>
       <c r="B129">
         <v>0.92671999999999999</v>
@@ -7038,7 +7063,7 @@
     <row r="130" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A130">
         <f t="shared" si="3"/>
-        <v>2.5620000000000016</v>
+        <v>1.5480000000000012</v>
       </c>
       <c r="B130">
         <v>0.95408000000000004</v>
@@ -7053,7 +7078,7 @@
     <row r="131" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A131">
         <f t="shared" si="3"/>
-        <v>2.5820000000000016</v>
+        <v>1.5600000000000012</v>
       </c>
       <c r="B131">
         <v>0.16847999999999999</v>
@@ -7064,8 +7089,8 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A132">
-        <f t="shared" ref="A132:A185" si="4">A131+20*10^-3</f>
-        <v>2.6020000000000016</v>
+        <f t="shared" ref="A132:A184" si="4">A131+12*10^-3</f>
+        <v>1.5720000000000012</v>
       </c>
       <c r="B132">
         <v>6.8400000000000002E-2</v>
@@ -7077,7 +7102,7 @@
     <row r="133" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A133">
         <f t="shared" si="4"/>
-        <v>2.6220000000000017</v>
+        <v>1.5840000000000012</v>
       </c>
       <c r="B133">
         <v>9.6079999999999999E-2</v>
@@ -7092,7 +7117,7 @@
     <row r="134" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A134">
         <f t="shared" si="4"/>
-        <v>2.6420000000000017</v>
+        <v>1.5960000000000012</v>
       </c>
       <c r="B134">
         <v>0.1236</v>
@@ -7107,7 +7132,7 @@
     <row r="135" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A135">
         <f t="shared" si="4"/>
-        <v>2.6620000000000017</v>
+        <v>1.6080000000000012</v>
       </c>
       <c r="B135">
         <v>0.15064</v>
@@ -7122,7 +7147,7 @@
     <row r="136" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A136">
         <f t="shared" si="4"/>
-        <v>2.6820000000000017</v>
+        <v>1.6200000000000012</v>
       </c>
       <c r="B136">
         <v>0.17784</v>
@@ -7137,7 +7162,7 @@
     <row r="137" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A137">
         <f t="shared" si="4"/>
-        <v>2.7020000000000017</v>
+        <v>1.6320000000000012</v>
       </c>
       <c r="B137">
         <v>0.20535999999999999</v>
@@ -7152,7 +7177,7 @@
     <row r="138" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A138">
         <f t="shared" si="4"/>
-        <v>2.7220000000000018</v>
+        <v>1.6440000000000012</v>
       </c>
       <c r="B138">
         <v>0.23280000000000001</v>
@@ -7167,7 +7192,7 @@
     <row r="139" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A139">
         <f t="shared" si="4"/>
-        <v>2.7420000000000018</v>
+        <v>1.6560000000000012</v>
       </c>
       <c r="B139">
         <v>0.26024000000000003</v>
@@ -7182,7 +7207,7 @@
     <row r="140" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A140">
         <f t="shared" si="4"/>
-        <v>2.7620000000000018</v>
+        <v>1.6680000000000013</v>
       </c>
       <c r="B140">
         <v>0.28736</v>
@@ -7197,7 +7222,7 @@
     <row r="141" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A141">
         <f t="shared" si="4"/>
-        <v>2.7820000000000018</v>
+        <v>1.6800000000000013</v>
       </c>
       <c r="B141">
         <v>0.31447999999999998</v>
@@ -7212,7 +7237,7 @@
     <row r="142" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A142">
         <f t="shared" si="4"/>
-        <v>2.8020000000000018</v>
+        <v>1.6920000000000013</v>
       </c>
       <c r="B142">
         <v>0.34160000000000001</v>
@@ -7227,7 +7252,7 @@
     <row r="143" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A143">
         <f t="shared" si="4"/>
-        <v>2.8220000000000018</v>
+        <v>1.7040000000000013</v>
       </c>
       <c r="B143">
         <v>0.36880000000000002</v>
@@ -7242,7 +7267,7 @@
     <row r="144" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A144">
         <f t="shared" si="4"/>
-        <v>2.8420000000000019</v>
+        <v>1.7160000000000013</v>
       </c>
       <c r="B144">
         <v>0.39584000000000003</v>
@@ -7257,7 +7282,7 @@
     <row r="145" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A145">
         <f t="shared" si="4"/>
-        <v>2.8620000000000019</v>
+        <v>1.7280000000000013</v>
       </c>
       <c r="B145">
         <v>0.42255999999999999</v>
@@ -7272,7 +7297,7 @@
     <row r="146" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A146">
         <f t="shared" si="4"/>
-        <v>2.8820000000000019</v>
+        <v>1.7400000000000013</v>
       </c>
       <c r="B146">
         <v>0.45016</v>
@@ -7287,7 +7312,7 @@
     <row r="147" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A147">
         <f t="shared" si="4"/>
-        <v>2.9020000000000019</v>
+        <v>1.7520000000000013</v>
       </c>
       <c r="B147">
         <v>0.47743999999999998</v>
@@ -7302,7 +7327,7 @@
     <row r="148" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A148">
         <f t="shared" si="4"/>
-        <v>2.9220000000000019</v>
+        <v>1.7640000000000013</v>
       </c>
       <c r="B148">
         <v>0.50463999999999998</v>
@@ -7317,7 +7342,7 @@
     <row r="149" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A149">
         <f t="shared" si="4"/>
-        <v>2.9420000000000019</v>
+        <v>1.7760000000000014</v>
       </c>
       <c r="B149">
         <v>0.53136000000000005</v>
@@ -7332,7 +7357,7 @@
     <row r="150" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A150">
         <f t="shared" si="4"/>
-        <v>2.962000000000002</v>
+        <v>1.7880000000000014</v>
       </c>
       <c r="B150">
         <v>0.55808000000000002</v>
@@ -7347,7 +7372,7 @@
     <row r="151" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A151">
         <f t="shared" si="4"/>
-        <v>2.982000000000002</v>
+        <v>1.8000000000000014</v>
       </c>
       <c r="B151">
         <v>0.58496000000000004</v>
@@ -7362,7 +7387,7 @@
     <row r="152" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A152">
         <f t="shared" si="4"/>
-        <v>3.002000000000002</v>
+        <v>1.8120000000000014</v>
       </c>
       <c r="B152">
         <v>0.61240000000000006</v>
@@ -7377,7 +7402,7 @@
     <row r="153" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A153">
         <f t="shared" si="4"/>
-        <v>3.022000000000002</v>
+        <v>1.8240000000000014</v>
       </c>
       <c r="B153">
         <v>0.63951999999999998</v>
@@ -7392,7 +7417,7 @@
     <row r="154" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A154">
         <f t="shared" si="4"/>
-        <v>3.042000000000002</v>
+        <v>1.8360000000000014</v>
       </c>
       <c r="B154">
         <v>0.66703999999999997</v>
@@ -7407,7 +7432,7 @@
     <row r="155" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A155">
         <f t="shared" si="4"/>
-        <v>3.0620000000000021</v>
+        <v>1.8480000000000014</v>
       </c>
       <c r="B155">
         <v>0.69688000000000005</v>
@@ -7422,7 +7447,7 @@
     <row r="156" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A156">
         <f t="shared" si="4"/>
-        <v>3.0820000000000021</v>
+        <v>1.8600000000000014</v>
       </c>
       <c r="B156">
         <v>0.72407999999999995</v>
@@ -7437,7 +7462,7 @@
     <row r="157" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A157">
         <f t="shared" si="4"/>
-        <v>3.1020000000000021</v>
+        <v>1.8720000000000014</v>
       </c>
       <c r="B157">
         <v>0.75119999999999998</v>
@@ -7452,7 +7477,7 @@
     <row r="158" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A158">
         <f t="shared" si="4"/>
-        <v>3.1220000000000021</v>
+        <v>1.8840000000000015</v>
       </c>
       <c r="B158">
         <v>0.77856000000000003</v>
@@ -7467,7 +7492,7 @@
     <row r="159" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A159">
         <f t="shared" si="4"/>
-        <v>3.1420000000000021</v>
+        <v>1.8960000000000015</v>
       </c>
       <c r="B159">
         <v>0.80576000000000003</v>
@@ -7482,7 +7507,7 @@
     <row r="160" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A160">
         <f t="shared" si="4"/>
-        <v>3.1620000000000021</v>
+        <v>1.9080000000000015</v>
       </c>
       <c r="B160">
         <v>0.83223999999999998</v>
@@ -7497,7 +7522,7 @@
     <row r="161" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A161">
         <f t="shared" si="4"/>
-        <v>3.1820000000000022</v>
+        <v>1.9200000000000015</v>
       </c>
       <c r="B161">
         <v>0.85928000000000004</v>
@@ -7512,7 +7537,7 @@
     <row r="162" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A162">
         <f t="shared" si="4"/>
-        <v>3.2020000000000022</v>
+        <v>1.9320000000000015</v>
       </c>
       <c r="B162">
         <v>0.88615999999999995</v>
@@ -7527,7 +7552,7 @@
     <row r="163" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A163">
         <f t="shared" si="4"/>
-        <v>3.2220000000000022</v>
+        <v>1.9440000000000015</v>
       </c>
       <c r="B163">
         <v>0.91303999999999996</v>
@@ -7542,7 +7567,7 @@
     <row r="164" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A164">
         <f t="shared" si="4"/>
-        <v>3.2420000000000022</v>
+        <v>1.9560000000000015</v>
       </c>
       <c r="B164">
         <v>0.94</v>
@@ -7557,7 +7582,7 @@
     <row r="165" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A165">
         <f t="shared" si="4"/>
-        <v>3.2620000000000022</v>
+        <v>1.9680000000000015</v>
       </c>
       <c r="B165">
         <v>0.79432000000000003</v>
@@ -7569,7 +7594,7 @@
     <row r="166" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A166">
         <f t="shared" si="4"/>
-        <v>3.2820000000000022</v>
+        <v>1.9800000000000015</v>
       </c>
       <c r="B166">
         <v>5.3760000000000002E-2</v>
@@ -7581,7 +7606,7 @@
     <row r="167" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A167">
         <f t="shared" si="4"/>
-        <v>3.3020000000000023</v>
+        <v>1.9920000000000015</v>
       </c>
       <c r="B167">
         <v>8.0960000000000004E-2</v>
@@ -7596,7 +7621,7 @@
     <row r="168" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A168">
         <f t="shared" si="4"/>
-        <v>3.3220000000000023</v>
+        <v>2.0040000000000013</v>
       </c>
       <c r="B168">
         <v>0.10888</v>
@@ -7611,7 +7636,7 @@
     <row r="169" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A169">
         <f t="shared" si="4"/>
-        <v>3.3420000000000023</v>
+        <v>2.0160000000000013</v>
       </c>
       <c r="B169">
         <v>0.13624</v>
@@ -7626,7 +7651,7 @@
     <row r="170" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A170">
         <f t="shared" si="4"/>
-        <v>3.3620000000000023</v>
+        <v>2.0280000000000014</v>
       </c>
       <c r="B170">
         <v>0.16328000000000001</v>
@@ -7641,7 +7666,7 @@
     <row r="171" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A171">
         <f t="shared" si="4"/>
-        <v>3.3820000000000023</v>
+        <v>2.0400000000000014</v>
       </c>
       <c r="B171">
         <v>0.19064</v>
@@ -7656,7 +7681,7 @@
     <row r="172" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A172">
         <f t="shared" si="4"/>
-        <v>3.4020000000000024</v>
+        <v>2.0520000000000014</v>
       </c>
       <c r="B172">
         <v>0.21848000000000001</v>
@@ -7671,7 +7696,7 @@
     <row r="173" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A173">
         <f t="shared" si="4"/>
-        <v>3.4220000000000024</v>
+        <v>2.0640000000000014</v>
       </c>
       <c r="B173">
         <v>0.24584</v>
@@ -7686,7 +7711,7 @@
     <row r="174" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A174">
         <f t="shared" si="4"/>
-        <v>3.4420000000000024</v>
+        <v>2.0760000000000014</v>
       </c>
       <c r="B174">
         <v>0.27279999999999999</v>
@@ -7701,7 +7726,7 @@
     <row r="175" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A175">
         <f t="shared" si="4"/>
-        <v>3.4620000000000024</v>
+        <v>2.0880000000000014</v>
       </c>
       <c r="B175">
         <v>0.30031999999999998</v>
@@ -7716,7 +7741,7 @@
     <row r="176" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A176">
         <f t="shared" si="4"/>
-        <v>3.4820000000000024</v>
+        <v>2.1000000000000014</v>
       </c>
       <c r="B176">
         <v>0.32712000000000002</v>
@@ -7731,7 +7756,7 @@
     <row r="177" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A177">
         <f t="shared" si="4"/>
-        <v>3.5020000000000024</v>
+        <v>2.1120000000000014</v>
       </c>
       <c r="B177">
         <v>0.35432000000000002</v>
@@ -7746,7 +7771,7 @@
     <row r="178" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A178">
         <f t="shared" si="4"/>
-        <v>3.5220000000000025</v>
+        <v>2.1240000000000014</v>
       </c>
       <c r="B178">
         <v>0.38144</v>
@@ -7761,7 +7786,7 @@
     <row r="179" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A179">
         <f t="shared" si="4"/>
-        <v>3.5420000000000025</v>
+        <v>2.1360000000000015</v>
       </c>
       <c r="B179">
         <v>0.40848000000000001</v>
@@ -7776,7 +7801,7 @@
     <row r="180" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A180">
         <f t="shared" si="4"/>
-        <v>3.5620000000000025</v>
+        <v>2.1480000000000015</v>
       </c>
       <c r="B180">
         <v>0.43536000000000002</v>
@@ -7791,7 +7816,7 @@
     <row r="181" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A181">
         <f t="shared" si="4"/>
-        <v>3.5820000000000025</v>
+        <v>2.1600000000000015</v>
       </c>
       <c r="B181">
         <v>0.46295999999999998</v>
@@ -7806,7 +7831,7 @@
     <row r="182" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A182">
         <f t="shared" si="4"/>
-        <v>3.6020000000000025</v>
+        <v>2.1720000000000015</v>
       </c>
       <c r="B182">
         <v>0.49024000000000001</v>
@@ -7821,7 +7846,7 @@
     <row r="183" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A183">
         <f t="shared" si="4"/>
-        <v>3.6220000000000026</v>
+        <v>2.1840000000000015</v>
       </c>
       <c r="B183">
         <v>0.51759999999999995</v>
@@ -7836,7 +7861,7 @@
     <row r="184" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A184">
         <f t="shared" si="4"/>
-        <v>3.6420000000000026</v>
+        <v>2.1960000000000015</v>
       </c>
       <c r="B184">
         <v>0.54471999999999998</v>
@@ -7849,10 +7874,6 @@
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A185">
-        <f t="shared" si="4"/>
-        <v>3.6620000000000026</v>
-      </c>
       <c r="B185">
         <v>0.57447999999999999</v>
       </c>

</xml_diff>